<commit_message>
Corretti fogli excel Synapse Value e Synapse Workflow
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/accreditamento-checklist_V4.2.xlsx
+++ b/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/accreditamento-checklist_V4.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmontel/Documents/dev/FSE/cda-fse/src/test/resources/accreditation/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmontel/Documents/dev/FSE/it-fse-accreditamento/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C87076FE-56DE-C64F-A7E5-360141491116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF3C9D2-3125-C74A-A04B-D3CE631C9594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="22840" windowWidth="30640" windowHeight="19380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="22840" windowWidth="30640" windowHeight="19380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="901" uniqueCount="404">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1918,42 +1918,6 @@
     <t>A fronte di un timeout nell'invio viene generata una Exception che viene gestita dall'applicativo</t>
   </si>
   <si>
-    <t>Il campo person_id non è stato compilato. Viene generato un errore di token di tipo: "/msg/jwt-validation", che dice:  "Il campo person_id non è valorizzato"</t>
-  </si>
-  <si>
-    <t>E'stato valorizzato il campo  purpose_of_use con il valore UNKNOWN. Viene generatoun  errore di token di tipo: "/msg/jwt-validation", che dice "Il campo purpose_of_use non è corretto"</t>
-  </si>
-  <si>
-    <t>E' stato immesso il codice fiscale errato: "dxxrxx46R24G729U". Viene generato l'errore: "Errore-46| codice fiscale 'dxxrxx46R24G729U' cittadino ed operatore: 16 cifre [A-Z0-9]{16}"</t>
-  </si>
-  <si>
-    <t>E'stato inserito un confidentialityCode code="R". Viene generato l'errore: "ERRORE-6| L'elemento  'confidentialityCode' di ClinicalDocument DEVE avere  l'attributo @code  valorizzato con 'N' o 'V',  il suo @codeSystem  con '2.16.840.1.113883.5.25'"</t>
-  </si>
-  <si>
-    <t>Viene omesso l'elemento city e si ottiene l'errore: "ERRORE-11| L'elemento ClinicalDocument/recordTarget/patientRole/addr DEVE riportare i suoi sotto-elementi 'country', 'city' e 'streetAddressLine'."</t>
-  </si>
-  <si>
-    <t>Viene omesso l'elemento given e si ottiene l'errore "ERRORE-14| L'elemento ClinicalDocument/recordTaget/patientRole/patient/name DEVE riportare gli elementi 'given' e 'family'"</t>
-  </si>
-  <si>
-    <t>Viene popolato il campo code con il valore "NB". Si ottiene l'errore di vocabolario: "Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.1 v2.1.0, Codes: NB]"</t>
-  </si>
-  <si>
-    <t>Viene valorizzato il campo code con il valore non previsto: "FSE-Test-11". Viene generato l'errore: "ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR'"</t>
-  </si>
-  <si>
-    <t>Viene popolato il campo priorityCode con il valore non previsto: "Test-12". Viene generato l'errore: "ERRORE-39| ClinicalDocument/infulfillmentOf/order/priorityCode DEVE avere l'attributo code valorizzato con uno dei seguenti valori: 'R'|'P'|'UR'|'EM'"</t>
-  </si>
-  <si>
-    <t>Nella sezione inFulfillmentOf viene omesso l'elemento order/id. Viene generato un errore sintattico dove è richiesto la valorizzazione del campo id</t>
-  </si>
-  <si>
-    <t>Viene omesso il contenuto del campo code relativo alle sezioni degli esami eseguiti. Viene generato un errore sintattico che notifica che il valore '' non rispetta il pattern '[^\s]+'</t>
-  </si>
-  <si>
-    <t>La sezione code=18782-3 contenente il referto non viene valorizzata. Vengono sollevati due errori: "[ERRORE-b4| Sezione Referto: DEVE essere presente la sezione "Referto".],[ERRORE-b5| Sezione Referto: La sezione deve contenere l'elemento 'text'.]"</t>
-  </si>
-  <si>
     <t>Il test non è supportato in quanto per l'utente non è possibile indicare quali precedenti esami eseguiti hanno contribuito alla formulazione del referto. L'utente può vederli ma non può selezionarli ai fini di quanto richiesto in questo contesto.</t>
   </si>
   <si>
@@ -1966,9 +1930,6 @@
     <t>Il test non può essere completamente validato in quanto l'applicazione non gestisce le codifiche LOINC relative al quesito diagnostico.</t>
   </si>
   <si>
-    <t>Il campo code viene valorizzato con il valore non previsto "FSE-Test-11". Viene generato l'errore :"ERRORE-40| L'elemento ClinicalDocument/documentationOf/serviceEvent deve contenere l'elemento code e DEVE valorizzare il suo attributo code con uno dei seguenti valori: 'PROG'|'DIR'|'RAD_PROG|'RAD_DIR'"</t>
-  </si>
-  <si>
     <t>Riportato errore validazione</t>
   </si>
   <si>
@@ -2116,69 +2077,6 @@
     <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.54c3707c2e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>a946949fbe0edd60</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:57.34Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.964c99cd5b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>49b43449a783a86e</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:58.945Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.8b96244c45^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>702732cb4a5a1527</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:11:00.576Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.660ef6ee73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>7206f0fefb149423</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:11:02.29Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.55db3d62e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>02e4d2be02bd501c</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:11:03.988Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.867c5dffc2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8085a7ec8d178a30</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:11:05.634Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.06875d318f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>0909583edbb75b57</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:11:07.331Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.a9bc8fa94a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>38f3d4faba4a1e98</t>
   </si>
   <si>
@@ -2198,9 +2096,6 @@
   </si>
   <si>
     <t>Viene sollevato un errore relativo alla validazione del token JWT in quanto vengono omessi tutti gli identificativi del paziente compreso il codice fiscale che invece è mandatorio per la validazione del token JWT. Il test è stato modificato come richiesto da Irene Stacchiotti: "Buongiorno Marco, grazie per la segnalazione. Le chiediamo cortesemente di modificare il caso di test utilizzando il campo confidentialityCode invece del patientRole/id. Seguirà una versione aggiornata della documentazione. Grazie mille."</t>
-  </si>
-  <si>
-    <t>Il test è stato modificato come richiesto da Irene Stacchiotti in quanto la versione originale non è applicabile. E'stato quindi omesso il campo confidentialityCode ottenendo un errore sintattico che in definitiva contiene la stringa "'{\"urn:hl7-org:v3\":confidentialityCode}' is expected."</t>
   </si>
 </sst>
 </file>
@@ -4320,10 +4215,10 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I43" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="E19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L76" sqref="L76"/>
+      <selection pane="bottomRight" activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4374,7 +4269,7 @@
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="51" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="D2" s="50"/>
       <c r="F2" s="26"/>
@@ -4910,13 +4805,13 @@
         <v>44981</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>363</v>
+        <v>350</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="I19" s="38" t="s">
-        <v>365</v>
+        <v>352</v>
       </c>
       <c r="J19" s="39" t="s">
         <v>84</v>
@@ -4954,13 +4849,13 @@
         <v>44981</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>366</v>
+        <v>353</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>367</v>
+        <v>354</v>
       </c>
       <c r="I20" s="38" t="s">
-        <v>368</v>
+        <v>355</v>
       </c>
       <c r="J20" s="39" t="s">
         <v>84</v>
@@ -4994,15 +4889,17 @@
       <c r="E21" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="37"/>
+      <c r="F21" s="37">
+        <v>44981</v>
+      </c>
       <c r="G21" s="38" t="s">
-        <v>369</v>
+        <v>356</v>
       </c>
       <c r="H21" s="38" t="s">
-        <v>370</v>
+        <v>357</v>
       </c>
       <c r="I21" s="38" t="s">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="J21" s="39" t="s">
         <v>84</v>
@@ -5036,15 +4933,17 @@
       <c r="E22" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="37"/>
+      <c r="F22" s="37">
+        <v>44981</v>
+      </c>
       <c r="G22" s="38" t="s">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="H22" s="38" t="s">
-        <v>373</v>
+        <v>360</v>
       </c>
       <c r="I22" s="38" t="s">
-        <v>374</v>
+        <v>361</v>
       </c>
       <c r="J22" s="39" t="s">
         <v>321</v>
@@ -5556,28 +5455,28 @@
       <c r="E37" s="36" t="s">
         <v>88</v>
       </c>
-      <c r="F37" s="37"/>
+      <c r="F37" s="37">
+        <v>44981</v>
+      </c>
       <c r="G37" s="38" t="s">
-        <v>375</v>
+        <v>362</v>
       </c>
       <c r="H37" s="38" t="s">
-        <v>376</v>
+        <v>363</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="J37" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K37" s="39" t="s">
-        <v>344</v>
-      </c>
+      <c r="K37" s="39"/>
       <c r="L37" s="39"/>
       <c r="M37" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N37" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O37" s="39"/>
       <c r="P37" s="39"/>
@@ -5774,28 +5673,28 @@
       <c r="E43" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="F43" s="37"/>
+      <c r="F43" s="37">
+        <v>44981</v>
+      </c>
       <c r="G43" s="38" t="s">
-        <v>379</v>
+        <v>366</v>
       </c>
       <c r="H43" s="38" t="s">
-        <v>378</v>
+        <v>365</v>
       </c>
       <c r="I43" s="38" t="s">
-        <v>377</v>
+        <v>364</v>
       </c>
       <c r="J43" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K43" s="39" t="s">
-        <v>345</v>
-      </c>
+      <c r="K43" s="39"/>
       <c r="L43" s="39"/>
       <c r="M43" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N43" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O43" s="39"/>
       <c r="P43" s="39"/>
@@ -5996,7 +5895,9 @@
       <c r="E49" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="F49" s="37"/>
+      <c r="F49" s="37">
+        <v>44981</v>
+      </c>
       <c r="G49" s="38"/>
       <c r="H49" s="38"/>
       <c r="I49" s="38"/>
@@ -6009,7 +5910,7 @@
         <v>84</v>
       </c>
       <c r="N49" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O49" s="39"/>
       <c r="P49" s="39" t="s">
@@ -6880,7 +6781,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="128" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="34">
         <v>74</v>
       </c>
@@ -6930,35 +6831,35 @@
       <c r="E76" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="F76" s="37"/>
+      <c r="F76" s="37">
+        <v>44981</v>
+      </c>
       <c r="G76" s="38" t="s">
-        <v>434</v>
+        <v>400</v>
       </c>
       <c r="H76" s="38" t="s">
-        <v>435</v>
+        <v>401</v>
       </c>
       <c r="I76" s="38" t="s">
-        <v>436</v>
+        <v>402</v>
       </c>
       <c r="J76" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K76" s="39" t="s">
-        <v>438</v>
-      </c>
+      <c r="K76" s="39"/>
       <c r="L76" s="39"/>
       <c r="M76" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N76" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O76" s="39"/>
       <c r="P76" s="39"/>
       <c r="Q76" s="39"/>
       <c r="R76" s="42"/>
       <c r="S76" s="46" t="s">
-        <v>437</v>
+        <v>403</v>
       </c>
       <c r="T76" s="44" t="s">
         <v>330</v>
@@ -6980,28 +6881,28 @@
       <c r="E77" s="36" t="s">
         <v>163</v>
       </c>
-      <c r="F77" s="37"/>
+      <c r="F77" s="37">
+        <v>44981</v>
+      </c>
       <c r="G77" s="38" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="H77" s="38" t="s">
-        <v>381</v>
+        <v>368</v>
       </c>
       <c r="I77" s="38" t="s">
-        <v>382</v>
+        <v>369</v>
       </c>
       <c r="J77" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K77" s="39" t="s">
-        <v>346</v>
-      </c>
+      <c r="K77" s="39"/>
       <c r="L77" s="39"/>
       <c r="M77" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N77" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O77" s="39"/>
       <c r="P77" s="39"/>
@@ -7028,28 +6929,28 @@
       <c r="E78" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="F78" s="37"/>
+      <c r="F78" s="37">
+        <v>44981</v>
+      </c>
       <c r="G78" s="38" t="s">
-        <v>383</v>
+        <v>370</v>
       </c>
       <c r="H78" s="38" t="s">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="I78" s="38" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="J78" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K78" s="39" t="s">
-        <v>347</v>
-      </c>
+      <c r="K78" s="39"/>
       <c r="L78" s="39"/>
       <c r="M78" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N78" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O78" s="39"/>
       <c r="P78" s="39"/>
@@ -7076,28 +6977,28 @@
       <c r="E79" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="F79" s="37"/>
+      <c r="F79" s="37">
+        <v>44981</v>
+      </c>
       <c r="G79" s="38" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="H79" s="38" t="s">
-        <v>387</v>
+        <v>374</v>
       </c>
       <c r="I79" s="38" t="s">
-        <v>388</v>
+        <v>375</v>
       </c>
       <c r="J79" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K79" s="39" t="s">
-        <v>348</v>
-      </c>
+      <c r="K79" s="39"/>
       <c r="L79" s="39"/>
       <c r="M79" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N79" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O79" s="39"/>
       <c r="P79" s="39"/>
@@ -7124,28 +7025,28 @@
       <c r="E80" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="F80" s="37"/>
+      <c r="F80" s="37">
+        <v>44981</v>
+      </c>
       <c r="G80" s="38" t="s">
-        <v>389</v>
+        <v>376</v>
       </c>
       <c r="H80" s="38" t="s">
-        <v>390</v>
+        <v>377</v>
       </c>
       <c r="I80" s="38" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="J80" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K80" s="39" t="s">
-        <v>349</v>
-      </c>
+      <c r="K80" s="39"/>
       <c r="L80" s="39"/>
       <c r="M80" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N80" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O80" s="39"/>
       <c r="P80" s="39"/>
@@ -7172,28 +7073,28 @@
       <c r="E81" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="F81" s="37"/>
+      <c r="F81" s="37">
+        <v>44981</v>
+      </c>
       <c r="G81" s="38" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="H81" s="38" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="I81" s="38" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
       <c r="J81" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K81" s="39" t="s">
-        <v>350</v>
-      </c>
+      <c r="K81" s="39"/>
       <c r="L81" s="39"/>
       <c r="M81" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N81" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O81" s="39"/>
       <c r="P81" s="39"/>
@@ -7220,28 +7121,28 @@
       <c r="E82" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="F82" s="37"/>
+      <c r="F82" s="37">
+        <v>44981</v>
+      </c>
       <c r="G82" s="38" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="H82" s="38" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="I82" s="38" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="J82" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K82" s="39" t="s">
-        <v>351</v>
-      </c>
+      <c r="K82" s="39"/>
       <c r="L82" s="39"/>
       <c r="M82" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N82" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O82" s="39"/>
       <c r="P82" s="39"/>
@@ -7268,28 +7169,28 @@
       <c r="E83" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="F83" s="37"/>
+      <c r="F83" s="37">
+        <v>44981</v>
+      </c>
       <c r="G83" s="38" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="H83" s="38" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="I83" s="38" t="s">
-        <v>400</v>
+        <v>387</v>
       </c>
       <c r="J83" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K83" s="39" t="s">
-        <v>352</v>
-      </c>
+      <c r="K83" s="39"/>
       <c r="L83" s="39"/>
       <c r="M83" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N83" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O83" s="39"/>
       <c r="P83" s="39"/>
@@ -7316,28 +7217,28 @@
       <c r="E84" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="F84" s="37"/>
+      <c r="F84" s="37">
+        <v>44981</v>
+      </c>
       <c r="G84" s="38" t="s">
-        <v>402</v>
+        <v>389</v>
       </c>
       <c r="H84" s="38" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="I84" s="38" t="s">
-        <v>403</v>
+        <v>390</v>
       </c>
       <c r="J84" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K84" s="39" t="s">
-        <v>353</v>
-      </c>
+      <c r="K84" s="39"/>
       <c r="L84" s="39"/>
       <c r="M84" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N84" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O84" s="39"/>
       <c r="P84" s="39"/>
@@ -7364,28 +7265,28 @@
       <c r="E85" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="F85" s="37"/>
+      <c r="F85" s="37">
+        <v>44981</v>
+      </c>
       <c r="G85" s="38" t="s">
-        <v>404</v>
+        <v>391</v>
       </c>
       <c r="H85" s="38" t="s">
-        <v>405</v>
+        <v>392</v>
       </c>
       <c r="I85" s="38" t="s">
-        <v>406</v>
+        <v>393</v>
       </c>
       <c r="J85" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K85" s="39" t="s">
-        <v>354</v>
-      </c>
+      <c r="K85" s="39"/>
       <c r="L85" s="39"/>
       <c r="M85" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N85" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O85" s="39"/>
       <c r="P85" s="39"/>
@@ -7412,28 +7313,28 @@
       <c r="E86" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="F86" s="37"/>
+      <c r="F86" s="37">
+        <v>44981</v>
+      </c>
       <c r="G86" s="38" t="s">
-        <v>408</v>
+        <v>395</v>
       </c>
       <c r="H86" s="38" t="s">
-        <v>407</v>
+        <v>394</v>
       </c>
       <c r="I86" s="38" t="s">
-        <v>409</v>
+        <v>396</v>
       </c>
       <c r="J86" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K86" s="39" t="s">
-        <v>355</v>
-      </c>
+      <c r="K86" s="39"/>
       <c r="L86" s="39"/>
       <c r="M86" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N86" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O86" s="39"/>
       <c r="P86" s="39"/>
@@ -7460,21 +7361,17 @@
       <c r="E87" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="F87" s="37"/>
-      <c r="G87" s="38" t="s">
-        <v>411</v>
-      </c>
-      <c r="H87" s="38" t="s">
-        <v>410</v>
-      </c>
-      <c r="I87" s="38" t="s">
-        <v>412</v>
-      </c>
+      <c r="F87" s="37">
+        <v>44981</v>
+      </c>
+      <c r="G87" s="38"/>
+      <c r="H87" s="38"/>
+      <c r="I87" s="38"/>
       <c r="J87" s="39" t="s">
         <v>321</v>
       </c>
       <c r="K87" s="39" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
       <c r="L87" s="39"/>
       <c r="M87" s="39" t="s">
@@ -7506,21 +7403,17 @@
       <c r="E88" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="F88" s="37"/>
-      <c r="G88" s="38" t="s">
-        <v>414</v>
-      </c>
-      <c r="H88" s="38" t="s">
-        <v>413</v>
-      </c>
-      <c r="I88" s="38" t="s">
-        <v>415</v>
-      </c>
+      <c r="F88" s="37">
+        <v>44981</v>
+      </c>
+      <c r="G88" s="38"/>
+      <c r="H88" s="38"/>
+      <c r="I88" s="38"/>
       <c r="J88" s="39" t="s">
         <v>321</v>
       </c>
       <c r="K88" s="39" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="L88" s="39"/>
       <c r="M88" s="39" t="s">
@@ -7552,21 +7445,17 @@
       <c r="E89" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="F89" s="37"/>
-      <c r="G89" s="38" t="s">
-        <v>417</v>
-      </c>
-      <c r="H89" s="38" t="s">
-        <v>416</v>
-      </c>
-      <c r="I89" s="38" t="s">
-        <v>418</v>
-      </c>
+      <c r="F89" s="37">
+        <v>44981</v>
+      </c>
+      <c r="G89" s="38"/>
+      <c r="H89" s="38"/>
+      <c r="I89" s="38"/>
       <c r="J89" s="39" t="s">
         <v>321</v>
       </c>
       <c r="K89" s="39" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="L89" s="39"/>
       <c r="M89" s="39" t="s">
@@ -7598,21 +7487,17 @@
       <c r="E90" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="F90" s="37"/>
-      <c r="G90" s="38" t="s">
-        <v>420</v>
-      </c>
-      <c r="H90" s="38" t="s">
-        <v>419</v>
-      </c>
-      <c r="I90" s="38" t="s">
-        <v>421</v>
-      </c>
+      <c r="F90" s="37">
+        <v>44981</v>
+      </c>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
+      <c r="I90" s="38"/>
       <c r="J90" s="39" t="s">
         <v>321</v>
       </c>
       <c r="K90" s="39" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="L90" s="39"/>
       <c r="M90" s="39" t="s">
@@ -7644,21 +7529,17 @@
       <c r="E91" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="F91" s="37"/>
-      <c r="G91" s="38" t="s">
-        <v>423</v>
-      </c>
-      <c r="H91" s="38" t="s">
-        <v>422</v>
-      </c>
-      <c r="I91" s="38" t="s">
-        <v>424</v>
-      </c>
+      <c r="F91" s="37">
+        <v>44981</v>
+      </c>
+      <c r="G91" s="38"/>
+      <c r="H91" s="38"/>
+      <c r="I91" s="38"/>
       <c r="J91" s="39" t="s">
         <v>321</v>
       </c>
       <c r="K91" s="39" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="L91" s="39"/>
       <c r="M91" s="39" t="s">
@@ -7690,21 +7571,17 @@
       <c r="E92" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="F92" s="37"/>
-      <c r="G92" s="38" t="s">
-        <v>426</v>
-      </c>
-      <c r="H92" s="38" t="s">
-        <v>425</v>
-      </c>
-      <c r="I92" s="38" t="s">
-        <v>427</v>
-      </c>
+      <c r="F92" s="37">
+        <v>44981</v>
+      </c>
+      <c r="G92" s="38"/>
+      <c r="H92" s="38"/>
+      <c r="I92" s="38"/>
       <c r="J92" s="39" t="s">
         <v>321</v>
       </c>
       <c r="K92" s="39" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="L92" s="39"/>
       <c r="M92" s="39" t="s">
@@ -7736,21 +7613,17 @@
       <c r="E93" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="F93" s="37"/>
-      <c r="G93" s="38" t="s">
-        <v>429</v>
-      </c>
-      <c r="H93" s="38" t="s">
-        <v>428</v>
-      </c>
-      <c r="I93" s="38" t="s">
-        <v>430</v>
-      </c>
+      <c r="F93" s="37">
+        <v>44981</v>
+      </c>
+      <c r="G93" s="38"/>
+      <c r="H93" s="38"/>
+      <c r="I93" s="38"/>
       <c r="J93" s="39" t="s">
         <v>321</v>
       </c>
       <c r="K93" s="39" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
       <c r="L93" s="39"/>
       <c r="M93" s="39" t="s">
@@ -7782,28 +7655,28 @@
       <c r="E94" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="F94" s="37"/>
+      <c r="F94" s="37">
+        <v>44981</v>
+      </c>
       <c r="G94" s="38" t="s">
-        <v>432</v>
+        <v>398</v>
       </c>
       <c r="H94" s="38" t="s">
-        <v>431</v>
+        <v>397</v>
       </c>
       <c r="I94" s="38" t="s">
-        <v>433</v>
+        <v>399</v>
       </c>
       <c r="J94" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="K94" s="39" t="s">
-        <v>360</v>
-      </c>
+      <c r="K94" s="39"/>
       <c r="L94" s="39"/>
       <c r="M94" s="39" t="s">
         <v>84</v>
       </c>
       <c r="N94" s="39" t="s">
-        <v>361</v>
+        <v>348</v>
       </c>
       <c r="O94" s="39"/>
       <c r="P94" s="39"/>
@@ -26189,6 +26062,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -26419,7 +26303,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -26428,18 +26312,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26458,27 +26348,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Cancellato campo F per applicabilità NO
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/accreditamento-checklist_V4.2.xlsx
+++ b/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/accreditamento-checklist_V4.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmontel/Documents/dev/FSE/it-fse-accreditamento/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E66D22-92A2-3C4D-A421-EA39C661E4E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED403B2-60BE-4843-B2EC-C92294AAB275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="22420" windowWidth="30640" windowHeight="19380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3580" yWindow="760" windowWidth="30980" windowHeight="20280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="403">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1955,15 +1955,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.ba4151a0d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:40.309Z[UTC]</t>
-  </si>
-  <si>
-    <t>9941622c2dbc0d75</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.de9033f617^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>2023-02-24T10:10:41.355Z[UTC]</t>
@@ -4220,11 +4211,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="I93" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="L76" sqref="L76:P76"/>
+      <selection pane="bottomRight" activeCell="F149" sqref="F149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4939,18 +4930,10 @@
       <c r="E22" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="37">
-        <v>44981</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>357</v>
-      </c>
-      <c r="H22" s="38" t="s">
-        <v>358</v>
-      </c>
-      <c r="I22" s="38" t="s">
-        <v>359</v>
-      </c>
+      <c r="F22" s="37"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
       <c r="J22" s="39" t="s">
         <v>321</v>
       </c>
@@ -5445,7 +5428,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="241" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="257" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="34">
         <v>31</v>
       </c>
@@ -5465,13 +5448,13 @@
         <v>44981</v>
       </c>
       <c r="G37" s="38" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H37" s="38" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="J37" s="39" t="s">
         <v>84</v>
@@ -5484,13 +5467,13 @@
         <v>84</v>
       </c>
       <c r="N37" s="39" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="O37" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P37" s="39" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="Q37" s="39"/>
       <c r="R37" s="42"/>
@@ -5669,7 +5652,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="241" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="257" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="34">
         <v>39</v>
       </c>
@@ -5689,13 +5672,13 @@
         <v>44981</v>
       </c>
       <c r="G43" s="38" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="H43" s="38" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="I43" s="38" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="J43" s="39" t="s">
         <v>84</v>
@@ -5708,13 +5691,13 @@
         <v>84</v>
       </c>
       <c r="N43" s="39" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="O43" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P43" s="39" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="Q43" s="39"/>
       <c r="R43" s="42"/>
@@ -5897,7 +5880,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="241" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" ht="257" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="34">
         <v>47</v>
       </c>
@@ -5930,13 +5913,13 @@
         <v>84</v>
       </c>
       <c r="N49" s="39" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="O49" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P49" s="39" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="Q49" s="39"/>
       <c r="R49" s="42" t="s">
@@ -6837,7 +6820,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="34">
         <v>75</v>
       </c>
@@ -6857,13 +6840,13 @@
         <v>44981</v>
       </c>
       <c r="G76" s="38" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="H76" s="38" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="I76" s="38" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="J76" s="39" t="s">
         <v>84</v>
@@ -6876,24 +6859,24 @@
         <v>84</v>
       </c>
       <c r="N76" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O76" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P76" s="42" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q76" s="39"/>
       <c r="R76" s="42"/>
       <c r="S76" s="46" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="T76" s="44" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="34">
         <v>76</v>
       </c>
@@ -6913,13 +6896,13 @@
         <v>44981</v>
       </c>
       <c r="G77" s="38" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="H77" s="38" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="I77" s="38" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="J77" s="39" t="s">
         <v>84</v>
@@ -6932,13 +6915,13 @@
         <v>84</v>
       </c>
       <c r="N77" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O77" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P77" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q77" s="39"/>
       <c r="R77" s="42"/>
@@ -6947,7 +6930,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="34">
         <v>77</v>
       </c>
@@ -6967,13 +6950,13 @@
         <v>44981</v>
       </c>
       <c r="G78" s="38" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="H78" s="38" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="I78" s="38" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="J78" s="39" t="s">
         <v>84</v>
@@ -6986,13 +6969,13 @@
         <v>84</v>
       </c>
       <c r="N78" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O78" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P78" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q78" s="39"/>
       <c r="R78" s="42"/>
@@ -7001,7 +6984,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="34">
         <v>78</v>
       </c>
@@ -7021,13 +7004,13 @@
         <v>44981</v>
       </c>
       <c r="G79" s="38" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="H79" s="38" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="I79" s="38" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="J79" s="39" t="s">
         <v>84</v>
@@ -7040,13 +7023,13 @@
         <v>84</v>
       </c>
       <c r="N79" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O79" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P79" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q79" s="39"/>
       <c r="R79" s="42"/>
@@ -7055,7 +7038,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="34">
         <v>79</v>
       </c>
@@ -7075,13 +7058,13 @@
         <v>44981</v>
       </c>
       <c r="G80" s="38" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="H80" s="38" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="I80" s="38" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="J80" s="39" t="s">
         <v>84</v>
@@ -7094,13 +7077,13 @@
         <v>84</v>
       </c>
       <c r="N80" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O80" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P80" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q80" s="39"/>
       <c r="R80" s="42"/>
@@ -7109,7 +7092,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="34">
         <v>80</v>
       </c>
@@ -7129,13 +7112,13 @@
         <v>44981</v>
       </c>
       <c r="G81" s="38" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="H81" s="38" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="I81" s="38" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="J81" s="39" t="s">
         <v>84</v>
@@ -7148,13 +7131,13 @@
         <v>84</v>
       </c>
       <c r="N81" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O81" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P81" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q81" s="39"/>
       <c r="R81" s="42"/>
@@ -7163,7 +7146,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="34">
         <v>81</v>
       </c>
@@ -7183,13 +7166,13 @@
         <v>44981</v>
       </c>
       <c r="G82" s="38" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="H82" s="38" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="I82" s="38" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="J82" s="39" t="s">
         <v>84</v>
@@ -7202,13 +7185,13 @@
         <v>84</v>
       </c>
       <c r="N82" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O82" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P82" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q82" s="39"/>
       <c r="R82" s="42"/>
@@ -7217,7 +7200,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="34">
         <v>82</v>
       </c>
@@ -7237,13 +7220,13 @@
         <v>44981</v>
       </c>
       <c r="G83" s="38" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H83" s="38" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="I83" s="38" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="J83" s="39" t="s">
         <v>84</v>
@@ -7256,13 +7239,13 @@
         <v>84</v>
       </c>
       <c r="N83" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O83" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P83" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q83" s="39"/>
       <c r="R83" s="42"/>
@@ -7271,7 +7254,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="34">
         <v>83</v>
       </c>
@@ -7291,13 +7274,13 @@
         <v>44981</v>
       </c>
       <c r="G84" s="38" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="H84" s="38" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I84" s="38" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="J84" s="39" t="s">
         <v>84</v>
@@ -7310,13 +7293,13 @@
         <v>84</v>
       </c>
       <c r="N84" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O84" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P84" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q84" s="39"/>
       <c r="R84" s="42"/>
@@ -7325,7 +7308,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="34">
         <v>84</v>
       </c>
@@ -7345,13 +7328,13 @@
         <v>44981</v>
       </c>
       <c r="G85" s="38" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H85" s="38" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="I85" s="38" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="J85" s="39" t="s">
         <v>84</v>
@@ -7364,13 +7347,13 @@
         <v>84</v>
       </c>
       <c r="N85" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O85" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P85" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q85" s="39"/>
       <c r="R85" s="42"/>
@@ -7379,7 +7362,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="34">
         <v>85</v>
       </c>
@@ -7399,13 +7382,13 @@
         <v>44981</v>
       </c>
       <c r="G86" s="38" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="H86" s="38" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="I86" s="38" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="J86" s="39" t="s">
         <v>84</v>
@@ -7418,13 +7401,13 @@
         <v>84</v>
       </c>
       <c r="N86" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O86" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P86" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q86" s="39"/>
       <c r="R86" s="42"/>
@@ -7449,9 +7432,7 @@
       <c r="E87" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="F87" s="37">
-        <v>44981</v>
-      </c>
+      <c r="F87" s="37"/>
       <c r="G87" s="38"/>
       <c r="H87" s="38"/>
       <c r="I87" s="38"/>
@@ -7491,9 +7472,7 @@
       <c r="E88" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="F88" s="37">
-        <v>44981</v>
-      </c>
+      <c r="F88" s="37"/>
       <c r="G88" s="38"/>
       <c r="H88" s="38"/>
       <c r="I88" s="38"/>
@@ -7533,9 +7512,7 @@
       <c r="E89" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="F89" s="37">
-        <v>44981</v>
-      </c>
+      <c r="F89" s="37"/>
       <c r="G89" s="38"/>
       <c r="H89" s="38"/>
       <c r="I89" s="38"/>
@@ -7575,9 +7552,7 @@
       <c r="E90" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="F90" s="37">
-        <v>44981</v>
-      </c>
+      <c r="F90" s="37"/>
       <c r="G90" s="38"/>
       <c r="H90" s="38"/>
       <c r="I90" s="38"/>
@@ -7617,9 +7592,7 @@
       <c r="E91" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="F91" s="37">
-        <v>44981</v>
-      </c>
+      <c r="F91" s="37"/>
       <c r="G91" s="38"/>
       <c r="H91" s="38"/>
       <c r="I91" s="38"/>
@@ -7659,9 +7632,7 @@
       <c r="E92" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="F92" s="37">
-        <v>44981</v>
-      </c>
+      <c r="F92" s="37"/>
       <c r="G92" s="38"/>
       <c r="H92" s="38"/>
       <c r="I92" s="38"/>
@@ -7701,9 +7672,7 @@
       <c r="E93" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="F93" s="37">
-        <v>44981</v>
-      </c>
+      <c r="F93" s="37"/>
       <c r="G93" s="38"/>
       <c r="H93" s="38"/>
       <c r="I93" s="38"/>
@@ -7727,7 +7696,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="272" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" ht="288" x14ac:dyDescent="0.2">
       <c r="A94" s="34">
         <v>93</v>
       </c>
@@ -7747,13 +7716,13 @@
         <v>44981</v>
       </c>
       <c r="G94" s="38" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="H94" s="38" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="I94" s="38" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="J94" s="39" t="s">
         <v>84</v>
@@ -7766,13 +7735,13 @@
         <v>84</v>
       </c>
       <c r="N94" s="39" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="O94" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P94" s="39" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="Q94" s="39"/>
       <c r="R94" s="42"/>
@@ -26387,15 +26356,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
@@ -26404,6 +26364,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26426,14 +26395,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -26450,6 +26411,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
A1#111FUJIFILM000 Correzione file, eliminati file test non supportati
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/accreditamento-checklist_V4.2.xlsx
+++ b/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/accreditamento-checklist_V4.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmontel/Documents/dev/FSE/it-fse-accreditamento/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmontel/Documents/dev/FSE/it-fse-accreditamento/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Workflow/4.33/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED403B2-60BE-4843-B2EC-C92294AAB275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A9B316-DF48-7743-B8B2-59120A0BB13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="760" windowWidth="30980" windowHeight="20280" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="-21100" windowWidth="30980" windowHeight="19700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="5" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="995" uniqueCount="400">
   <si>
     <t>PREREQUISITI</t>
   </si>
@@ -1903,196 +1903,187 @@
     <t xml:space="preserve">4) Se il test NON è applicabile la colonna APPLICABILITA' riporterà NO e dovrà essere compilata esclusivamente la colonna RAZIONALE DI APPLICABILITA' con le motivazioni per cui il test non è applicabile </t>
   </si>
   <si>
+    <t>subject_application_vendor: Fujifilm Italia S.p.A.</t>
+  </si>
+  <si>
+    <t>La sezione DICOM Object Catalog non è completa in quanto il sistema non ha accesso a tutto l'aggregato Study-&gt;Series-&gt;SOP Intences. La sezione "Precedenti esami eseguiti" non è completa in quanto l'utente non può selezionare gli esami precedenti eseguiti inerenti la refertazione corrente.</t>
+  </si>
+  <si>
+    <t>Il test non è supportato in quanto per l'utente non è possibile indicare quali precedenti esami eseguiti hanno contribuito alla formulazione del referto. L'utente può vederli ma non può selezionarli ai fini di quanto richiesto in questo contesto.</t>
+  </si>
+  <si>
+    <t>Il test non è supportato in quanto l'applicazione non ha accesso a tutto l'aggregato DICOM relativo allo studio in refertazione. Questo dato è dominio del PACS.</t>
+  </si>
+  <si>
+    <t>Il test non è supportato in quanto l'applicazione non gestisce la Storia Clinica così come previsto in questo contesto.</t>
+  </si>
+  <si>
+    <t>Il test non può essere completamente validato in quanto l'applicazione non gestisce le codifiche LOINC relative al quesito diagnostico.</t>
+  </si>
+  <si>
+    <t>Fujifilm Italia S.p.A.</t>
+  </si>
+  <si>
+    <t>UNKNOWN_WORKFLOW_ID</t>
+  </si>
+  <si>
+    <t>Viene sollevato un errore relativo alla validazione del token JWT in quanto vengono omessi tutti gli identificativi del paziente compreso il codice fiscale che invece è mandatorio per la validazione del token JWT. Il test è stato modificato come richiesto da Irene Stacchiotti: "Buongiorno Marco, grazie per la segnalazione. Le chiediamo cortesemente di modificare il caso di test utilizzando il campo confidentialityCode invece del patientRole/id. Seguirà una versione aggiornata della documentazione. Grazie mille."</t>
+  </si>
+  <si>
+    <t>Il record di refertazione viene bloccato nell'applicativo e visualizzato il messaggio di errore ricevuto da FSE.</t>
+  </si>
+  <si>
+    <t>Il caso viene gestito in back office con il seguente flusso: 1. Il record di refertazione viene bloccato sull'applicativo in uno stato di manutenzione. 2. Il caso di errore viene visualizzato nel modulo integrato gestione problematiche. 3. Un utente amministratore gestisce il caso, ed una volta risolto, il record di refertazione viene sbloccato e rimosso lo stato di manutenzione. 4. Il sistema sottopone nuovamente la richiesta di validazione a FSE</t>
+  </si>
+  <si>
+    <t>Si ha evidenza dell'errore tramite una icona sul record. I dettagli sono disponibili nel modulo integrato gestione problematiche richiamabile dal record stesso, dove viene visualizzato l'errore ricevuto da FSE.</t>
+  </si>
+  <si>
+    <t>Il caso viene gestito in back office con il seguente flusso: 1. Il record di refertazione viene bloccato sull'applicativo in uno stato di manutenzione. 2. Il caso di errore viene visualizzato nel modulo integrato gestione problematiche. 3. Un utente amministratore gestisce il caso, ed una volta risolto, il record di refertazione viene sbloccato e rimosso lo stato di manutenzione. 4. Il medico riceve una notifica automatica che riporta il problema risolto e lo invita a creare e firmare un addendum.</t>
+  </si>
+  <si>
+    <t>0aa8a2dba0809f3b</t>
+  </si>
+  <si>
+    <t>1913b3b338cd52b6</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.7181aa9472^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:21:00.216Z[UTC]</t>
+  </si>
+  <si>
+    <t>d42e7ede64b233fa</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:21:01.112Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.ec2538749c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>888cec3db845d0ad</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:41.589Z[UTC]</t>
+  </si>
+  <si>
+    <t>26f74d71e737ffef</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:59.317Z[UTC]</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:39.974Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.b7aa33d2df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>02f6c974efb65bfb</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:43.03Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.3ffdacb4e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>0a02c5f2c87933c7</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:44.48Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.6b1340eecf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>431c9c23de42236b</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:45.951Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.56b18f0ec4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>56ac2bc544261824</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:49.031Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.ecc1e2b6d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>068e88e8c55ae948</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:47.532Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.93961c8bc9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f320be9ee5698d0e</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:50.515Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.bc6f3ba2cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:51.907Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.a27d859a2d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5ff992ade30f769b</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:53.469Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.5eb7049956^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5d2a9cd381bb186d</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:54.915Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.1606281359^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2d2fb460d14af10e</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:56.441Z[UTC]</t>
+  </si>
+  <si>
+    <t>7681f7c242538a52</t>
+  </si>
+  <si>
+    <t>2023-04-11T14:20:57.889Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.a3139809b3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5a6c7cf5e8fb7a90</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.e439bcbd28^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
     <t>subject_application_id: Synapse Value</t>
   </si>
   <si>
-    <t>subject_application_vendor: Fujifilm Italia S.p.A.</t>
-  </si>
-  <si>
     <t>subject_application_version: 1.6</t>
-  </si>
-  <si>
-    <t>La sezione DICOM Object Catalog non è completa in quanto il sistema non ha accesso a tutto l'aggregato Study-&gt;Series-&gt;SOP Intences. La sezione "Precedenti esami eseguiti" non è completa in quanto l'utente non può selezionare gli esami precedenti eseguiti inerenti la refertazione corrente.</t>
-  </si>
-  <si>
-    <t>Il test non è supportato in quanto per l'utente non è possibile indicare quali precedenti esami eseguiti hanno contribuito alla formulazione del referto. L'utente può vederli ma non può selezionarli ai fini di quanto richiesto in questo contesto.</t>
-  </si>
-  <si>
-    <t>Il test non è supportato in quanto l'applicazione non ha accesso a tutto l'aggregato DICOM relativo allo studio in refertazione. Questo dato è dominio del PACS.</t>
-  </si>
-  <si>
-    <t>Il test non è supportato in quanto l'applicazione non gestisce la Storia Clinica così come previsto in questo contesto.</t>
-  </si>
-  <si>
-    <t>Il test non può essere completamente validato in quanto l'applicazione non gestisce le codifiche LOINC relative al quesito diagnostico.</t>
-  </si>
-  <si>
-    <t>Fujifilm Italia S.p.A.</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:35.836Z[UTC]</t>
-  </si>
-  <si>
-    <t>b54e4fd7fdf47b82</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.54342c2268^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:37.337Z[UTC]</t>
-  </si>
-  <si>
-    <t>54ee3ba0def34fcc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.2ee8ad61fa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:38.827Z[UTC]</t>
-  </si>
-  <si>
-    <t>bac359dfe0957993</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.ba4151a0d7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:41.355Z[UTC]</t>
-  </si>
-  <si>
-    <t>9b1f2ec72e088486</t>
-  </si>
-  <si>
-    <t>UNKNOWN_WORKFLOW_ID</t>
-  </si>
-  <si>
-    <t>0308c9f36badcea6</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:11:09.253Z[UTC]</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:43.386Z[UTC]</t>
-  </si>
-  <si>
-    <t>f309d4f6c71fffe9</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.a898b32ea4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:44.512Z[UTC]</t>
-  </si>
-  <si>
-    <t>66b4f3fc9d778670</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.cbbc008dfd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:45.55Z[UTC]</t>
-  </si>
-  <si>
-    <t>bc937dca28291215</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.5c52e20c28^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:48.223Z[UTC]</t>
-  </si>
-  <si>
-    <t>1788c85846c24f7d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.9d9cfbe1d3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>8efcc9d8697a5b32</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:49.865Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.427b477612^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>eef739567b69eba2</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:51.037Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.f0b3f220a0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>59d03514d5ab14ca</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:52.047Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.7061db4da7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>3750c9059a914aa7</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:53.725Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.be8498a838^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:54.691Z[UTC]</t>
-  </si>
-  <si>
-    <t>a65d16ea35ad3acc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.34f9e4d1f4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>980af3b3485ee4f2</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:10:55.637Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.54c3707c2e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>38f3d4faba4a1e98</t>
-  </si>
-  <si>
-    <t>2023-02-24T10:11:08.306Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.4c6a6f6b4e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-02-24T11:04:58.43Z[UTC]</t>
-  </si>
-  <si>
-    <t>060e5b22e40ca19d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.d19b13eb91^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>Viene sollevato un errore relativo alla validazione del token JWT in quanto vengono omessi tutti gli identificativi del paziente compreso il codice fiscale che invece è mandatorio per la validazione del token JWT. Il test è stato modificato come richiesto da Irene Stacchiotti: "Buongiorno Marco, grazie per la segnalazione. Le chiediamo cortesemente di modificare il caso di test utilizzando il campo confidentialityCode invece del patientRole/id. Seguirà una versione aggiornata della documentazione. Grazie mille."</t>
-  </si>
-  <si>
-    <t>Il record di refertazione viene bloccato nell'applicativo e visualizzato il messaggio di errore ricevuto da FSE.</t>
-  </si>
-  <si>
-    <t>Il caso viene gestito in back office con il seguente flusso: 1. Il record di refertazione viene bloccato sull'applicativo in uno stato di manutenzione. 2. Il caso di errore viene visualizzato nel modulo integrato gestione problematiche. 3. Un utente amministratore gestisce il caso, ed una volta risolto, il record di refertazione viene sbloccato e rimosso lo stato di manutenzione. 4. Il medico riceve una notifica automatica che riporta il problema risolto e lo invita a creare e firmare un addendum.</t>
-  </si>
-  <si>
-    <t>Si ha evidenza dell'errore tramite una icona sul record. I dettagli sono disponibili nel modulo integrato gestione problematiche richiamabile dal record stesso, dove viene visualizzato l'errore ricevuto da FSE.</t>
-  </si>
-  <si>
-    <t>Il caso viene gestito in back office con il seguente flusso: 1. Il record di refertazione viene bloccato sull'applicativo in uno stato di manutenzione. 2. Il caso di errore viene visualizzato nel modulo integrato gestione problematiche. 3. Un utente amministratore gestisce il caso, ed una volta risolto, il record di refertazione viene sbloccato e rimosso lo stato di manutenzione. 4. Il sistema sottopone nuovamente la richiesta di validazione a FSE</t>
   </si>
 </sst>
 </file>
@@ -3138,7 +3129,7 @@
   <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4211,11 +4202,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" ySplit="9" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F149" sqref="F149"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4224,7 +4215,7 @@
     <col min="2" max="2" width="15.1640625" style="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="44.1640625" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="104.6640625" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.33203125" style="25" customWidth="1"/>
     <col min="6" max="6" width="25.5" style="25" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" style="25" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.83203125" style="25" bestFit="1" customWidth="1"/>
@@ -4266,7 +4257,7 @@
       </c>
       <c r="B2" s="50"/>
       <c r="C2" s="51" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D2" s="50"/>
       <c r="F2" s="26"/>
@@ -4291,7 +4282,7 @@
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="58" t="s">
-        <v>339</v>
+        <v>398</v>
       </c>
       <c r="D3" s="50"/>
       <c r="F3" s="26"/>
@@ -4314,7 +4305,7 @@
       <c r="A4" s="54"/>
       <c r="B4" s="55"/>
       <c r="C4" s="58" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="29"/>
@@ -4338,7 +4329,7 @@
       <c r="A5" s="56"/>
       <c r="B5" s="57"/>
       <c r="C5" s="58" t="s">
-        <v>341</v>
+        <v>399</v>
       </c>
       <c r="D5" s="50"/>
       <c r="F5" s="26"/>
@@ -4476,7 +4467,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="34">
         <v>1</v>
       </c>
@@ -4510,7 +4501,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34">
         <v>2</v>
       </c>
@@ -4544,7 +4535,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="34">
         <v>3</v>
       </c>
@@ -4578,7 +4569,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="34">
         <v>4</v>
       </c>
@@ -4612,7 +4603,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="161" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34">
         <v>5</v>
       </c>
@@ -4646,7 +4637,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34">
         <v>6</v>
       </c>
@@ -4680,7 +4671,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34">
         <v>7</v>
       </c>
@@ -4714,7 +4705,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34">
         <v>8</v>
       </c>
@@ -4748,7 +4739,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>9</v>
       </c>
@@ -4782,7 +4773,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="145" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="34">
         <v>11</v>
       </c>
@@ -4799,16 +4790,16 @@
         <v>48</v>
       </c>
       <c r="F19" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G19" s="38" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="H19" s="38" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="I19" s="38" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="J19" s="39" t="s">
         <v>84</v>
@@ -4826,7 +4817,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="34">
         <v>12</v>
       </c>
@@ -4843,16 +4834,16 @@
         <v>50</v>
       </c>
       <c r="F20" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="I20" s="38" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="J20" s="39" t="s">
         <v>84</v>
@@ -4870,7 +4861,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="34">
         <v>13</v>
       </c>
@@ -4886,22 +4877,16 @@
       <c r="E21" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="37">
-        <v>44981</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>354</v>
-      </c>
-      <c r="H21" s="38" t="s">
-        <v>355</v>
-      </c>
-      <c r="I21" s="38" t="s">
-        <v>356</v>
-      </c>
+      <c r="F21" s="37"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
       <c r="J21" s="39" t="s">
-        <v>84</v>
-      </c>
-      <c r="K21" s="39"/>
+        <v>321</v>
+      </c>
+      <c r="K21" s="39" t="s">
+        <v>340</v>
+      </c>
       <c r="L21" s="39"/>
       <c r="M21" s="39"/>
       <c r="N21" s="39"/>
@@ -4914,7 +4899,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="34">
         <v>14</v>
       </c>
@@ -4938,7 +4923,7 @@
         <v>321</v>
       </c>
       <c r="K22" s="39" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="L22" s="39"/>
       <c r="M22" s="39"/>
@@ -4952,7 +4937,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="34">
         <v>16</v>
       </c>
@@ -4986,7 +4971,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="34">
         <v>17</v>
       </c>
@@ -5020,7 +5005,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="34">
         <v>18</v>
       </c>
@@ -5054,7 +5039,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="34">
         <v>19</v>
       </c>
@@ -5088,7 +5073,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34">
         <v>20</v>
       </c>
@@ -5122,7 +5107,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34">
         <v>21</v>
       </c>
@@ -5156,7 +5141,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34">
         <v>22</v>
       </c>
@@ -5190,7 +5175,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34">
         <v>23</v>
       </c>
@@ -5224,7 +5209,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="34">
         <v>24</v>
       </c>
@@ -5258,7 +5243,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="34">
         <v>25</v>
       </c>
@@ -5292,7 +5277,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="34">
         <v>26</v>
       </c>
@@ -5326,7 +5311,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="145" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="34">
         <v>27</v>
       </c>
@@ -5360,7 +5345,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" ht="193" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="34">
         <v>28</v>
       </c>
@@ -5394,7 +5379,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" ht="193" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="34">
         <v>29</v>
       </c>
@@ -5445,16 +5430,16 @@
         <v>88</v>
       </c>
       <c r="F37" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G37" s="38" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="H37" s="38" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="I37" s="38" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="J37" s="39" t="s">
         <v>84</v>
@@ -5467,13 +5452,13 @@
         <v>84</v>
       </c>
       <c r="N37" s="39" t="s">
-        <v>399</v>
+        <v>348</v>
       </c>
       <c r="O37" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P37" s="39" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="Q37" s="39"/>
       <c r="R37" s="42"/>
@@ -5482,7 +5467,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" ht="257" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="34">
         <v>33</v>
       </c>
@@ -5505,10 +5490,18 @@
       <c r="J38" s="39"/>
       <c r="K38" s="39"/>
       <c r="L38" s="39"/>
-      <c r="M38" s="39"/>
-      <c r="N38" s="39"/>
-      <c r="O38" s="39"/>
-      <c r="P38" s="39"/>
+      <c r="M38" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N38" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="O38" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P38" s="39" t="s">
+        <v>349</v>
+      </c>
       <c r="Q38" s="39"/>
       <c r="R38" s="42"/>
       <c r="S38" s="40"/>
@@ -5516,7 +5509,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" ht="257" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="34">
         <v>34</v>
       </c>
@@ -5539,10 +5532,18 @@
       <c r="J39" s="39"/>
       <c r="K39" s="39"/>
       <c r="L39" s="39"/>
-      <c r="M39" s="39"/>
-      <c r="N39" s="39"/>
-      <c r="O39" s="39"/>
-      <c r="P39" s="39"/>
+      <c r="M39" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N39" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="O39" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P39" s="39" t="s">
+        <v>349</v>
+      </c>
       <c r="Q39" s="39"/>
       <c r="R39" s="42"/>
       <c r="S39" s="40"/>
@@ -5550,7 +5551,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="113" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="34">
         <v>35</v>
       </c>
@@ -5573,10 +5574,18 @@
       <c r="J40" s="39"/>
       <c r="K40" s="39"/>
       <c r="L40" s="39"/>
-      <c r="M40" s="39"/>
-      <c r="N40" s="39"/>
-      <c r="O40" s="39"/>
-      <c r="P40" s="39"/>
+      <c r="M40" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N40" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O40" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P40" s="42" t="s">
+        <v>351</v>
+      </c>
       <c r="Q40" s="39"/>
       <c r="R40" s="42"/>
       <c r="S40" s="40"/>
@@ -5584,7 +5593,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="34">
         <v>36</v>
       </c>
@@ -5607,10 +5616,18 @@
       <c r="J41" s="39"/>
       <c r="K41" s="39"/>
       <c r="L41" s="39"/>
-      <c r="M41" s="39"/>
-      <c r="N41" s="39"/>
-      <c r="O41" s="39"/>
-      <c r="P41" s="39"/>
+      <c r="M41" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N41" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O41" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P41" s="39" t="s">
+        <v>351</v>
+      </c>
       <c r="Q41" s="39"/>
       <c r="R41" s="42"/>
       <c r="S41" s="40"/>
@@ -5618,7 +5635,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="34">
         <v>37</v>
       </c>
@@ -5641,10 +5658,18 @@
       <c r="J42" s="39"/>
       <c r="K42" s="39"/>
       <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="39"/>
-      <c r="P42" s="39"/>
+      <c r="M42" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N42" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O42" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P42" s="39" t="s">
+        <v>351</v>
+      </c>
       <c r="Q42" s="39"/>
       <c r="R42" s="42"/>
       <c r="S42" s="40"/>
@@ -5669,16 +5694,16 @@
         <v>100</v>
       </c>
       <c r="F43" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G43" s="38" t="s">
+        <v>362</v>
+      </c>
+      <c r="H43" s="38" t="s">
         <v>361</v>
       </c>
-      <c r="H43" s="38" t="s">
-        <v>360</v>
-      </c>
       <c r="I43" s="38" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="J43" s="39" t="s">
         <v>84</v>
@@ -5691,13 +5716,13 @@
         <v>84</v>
       </c>
       <c r="N43" s="39" t="s">
-        <v>399</v>
+        <v>348</v>
       </c>
       <c r="O43" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P43" s="39" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="Q43" s="39"/>
       <c r="R43" s="42"/>
@@ -5706,7 +5731,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="34">
         <v>41</v>
       </c>
@@ -5729,10 +5754,18 @@
       <c r="J44" s="39"/>
       <c r="K44" s="39"/>
       <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="39"/>
-      <c r="P44" s="39"/>
+      <c r="M44" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N44" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O44" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P44" s="39" t="s">
+        <v>351</v>
+      </c>
       <c r="Q44" s="39"/>
       <c r="R44" s="42"/>
       <c r="S44" s="40"/>
@@ -5740,7 +5773,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="34">
         <v>42</v>
       </c>
@@ -5763,10 +5796,18 @@
       <c r="J45" s="39"/>
       <c r="K45" s="39"/>
       <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="39"/>
-      <c r="O45" s="39"/>
-      <c r="P45" s="39"/>
+      <c r="M45" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N45" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O45" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P45" s="39" t="s">
+        <v>351</v>
+      </c>
       <c r="Q45" s="39"/>
       <c r="R45" s="42"/>
       <c r="S45" s="40"/>
@@ -5774,7 +5815,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="34">
         <v>43</v>
       </c>
@@ -5797,10 +5838,18 @@
       <c r="J46" s="39"/>
       <c r="K46" s="39"/>
       <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="39"/>
-      <c r="O46" s="39"/>
-      <c r="P46" s="39"/>
+      <c r="M46" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N46" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O46" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P46" s="39" t="s">
+        <v>351</v>
+      </c>
       <c r="Q46" s="39"/>
       <c r="R46" s="42"/>
       <c r="S46" s="40"/>
@@ -5808,7 +5857,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="49" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="34">
         <v>44</v>
       </c>
@@ -5831,10 +5880,18 @@
       <c r="J47" s="39"/>
       <c r="K47" s="39"/>
       <c r="L47" s="39"/>
-      <c r="M47" s="39"/>
-      <c r="N47" s="39"/>
-      <c r="O47" s="39"/>
-      <c r="P47" s="39"/>
+      <c r="M47" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N47" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O47" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P47" s="39" t="s">
+        <v>351</v>
+      </c>
       <c r="Q47" s="39"/>
       <c r="R47" s="42" t="s">
         <v>84</v>
@@ -5844,7 +5901,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="49" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="34">
         <v>45</v>
       </c>
@@ -5867,10 +5924,18 @@
       <c r="J48" s="39"/>
       <c r="K48" s="39"/>
       <c r="L48" s="39"/>
-      <c r="M48" s="39"/>
-      <c r="N48" s="39"/>
-      <c r="O48" s="39"/>
-      <c r="P48" s="39"/>
+      <c r="M48" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N48" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O48" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P48" s="39" t="s">
+        <v>351</v>
+      </c>
       <c r="Q48" s="39"/>
       <c r="R48" s="42" t="s">
         <v>84</v>
@@ -5897,7 +5962,7 @@
         <v>108</v>
       </c>
       <c r="F49" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G49" s="38"/>
       <c r="H49" s="38"/>
@@ -5913,13 +5978,13 @@
         <v>84</v>
       </c>
       <c r="N49" s="39" t="s">
-        <v>399</v>
+        <v>348</v>
       </c>
       <c r="O49" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P49" s="39" t="s">
-        <v>402</v>
+        <v>349</v>
       </c>
       <c r="Q49" s="39"/>
       <c r="R49" s="42" t="s">
@@ -5930,7 +5995,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="49" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="34">
         <v>49</v>
       </c>
@@ -5953,10 +6018,18 @@
       <c r="J50" s="39"/>
       <c r="K50" s="39"/>
       <c r="L50" s="39"/>
-      <c r="M50" s="39"/>
-      <c r="N50" s="39"/>
-      <c r="O50" s="39"/>
-      <c r="P50" s="39"/>
+      <c r="M50" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N50" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O50" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P50" s="39" t="s">
+        <v>351</v>
+      </c>
       <c r="Q50" s="39"/>
       <c r="R50" s="42" t="s">
         <v>84</v>
@@ -5966,7 +6039,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="49" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" ht="65" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="34">
         <v>50</v>
       </c>
@@ -5989,7 +6062,9 @@
       <c r="J51" s="39"/>
       <c r="K51" s="39"/>
       <c r="L51" s="39"/>
-      <c r="M51" s="39"/>
+      <c r="M51" s="39" t="s">
+        <v>321</v>
+      </c>
       <c r="N51" s="39"/>
       <c r="O51" s="39"/>
       <c r="P51" s="39"/>
@@ -6002,7 +6077,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="49" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" ht="65" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="34">
         <v>51</v>
       </c>
@@ -6025,7 +6100,9 @@
       <c r="J52" s="39"/>
       <c r="K52" s="39"/>
       <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
+      <c r="M52" s="39" t="s">
+        <v>321</v>
+      </c>
       <c r="N52" s="39"/>
       <c r="O52" s="39"/>
       <c r="P52" s="39"/>
@@ -6038,7 +6115,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="34">
         <v>52</v>
       </c>
@@ -6061,7 +6138,9 @@
       <c r="J53" s="39"/>
       <c r="K53" s="39"/>
       <c r="L53" s="39"/>
-      <c r="M53" s="39"/>
+      <c r="M53" s="39" t="s">
+        <v>321</v>
+      </c>
       <c r="N53" s="39"/>
       <c r="O53" s="39"/>
       <c r="P53" s="39"/>
@@ -6072,7 +6151,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="34">
         <v>53</v>
       </c>
@@ -6095,7 +6174,9 @@
       <c r="J54" s="39"/>
       <c r="K54" s="39"/>
       <c r="L54" s="39"/>
-      <c r="M54" s="39"/>
+      <c r="M54" s="39" t="s">
+        <v>321</v>
+      </c>
       <c r="N54" s="39"/>
       <c r="O54" s="39"/>
       <c r="P54" s="39"/>
@@ -6106,7 +6187,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="34">
         <v>54</v>
       </c>
@@ -6129,7 +6210,9 @@
       <c r="J55" s="39"/>
       <c r="K55" s="39"/>
       <c r="L55" s="39"/>
-      <c r="M55" s="39"/>
+      <c r="M55" s="39" t="s">
+        <v>321</v>
+      </c>
       <c r="N55" s="39"/>
       <c r="O55" s="39"/>
       <c r="P55" s="39"/>
@@ -6140,7 +6223,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="34">
         <v>55</v>
       </c>
@@ -6163,7 +6246,9 @@
       <c r="J56" s="39"/>
       <c r="K56" s="39"/>
       <c r="L56" s="39"/>
-      <c r="M56" s="39"/>
+      <c r="M56" s="39" t="s">
+        <v>321</v>
+      </c>
       <c r="N56" s="39"/>
       <c r="O56" s="39"/>
       <c r="P56" s="39"/>
@@ -6174,7 +6259,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="34">
         <v>56</v>
       </c>
@@ -6197,7 +6282,9 @@
       <c r="J57" s="39"/>
       <c r="K57" s="39"/>
       <c r="L57" s="39"/>
-      <c r="M57" s="39"/>
+      <c r="M57" s="39" t="s">
+        <v>321</v>
+      </c>
       <c r="N57" s="39"/>
       <c r="O57" s="39"/>
       <c r="P57" s="39"/>
@@ -6208,7 +6295,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="34">
         <v>57</v>
       </c>
@@ -6231,10 +6318,18 @@
       <c r="J58" s="39"/>
       <c r="K58" s="39"/>
       <c r="L58" s="39"/>
-      <c r="M58" s="39"/>
-      <c r="N58" s="39"/>
-      <c r="O58" s="39"/>
-      <c r="P58" s="39"/>
+      <c r="M58" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="N58" s="39" t="s">
+        <v>350</v>
+      </c>
+      <c r="O58" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="P58" s="39" t="s">
+        <v>351</v>
+      </c>
       <c r="Q58" s="39"/>
       <c r="R58" s="42"/>
       <c r="S58" s="40"/>
@@ -6242,7 +6337,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="34">
         <v>58</v>
       </c>
@@ -6276,7 +6371,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="34">
         <v>59</v>
       </c>
@@ -6310,7 +6405,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="34">
         <v>60</v>
       </c>
@@ -6344,7 +6439,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="34">
         <v>61</v>
       </c>
@@ -6378,7 +6473,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="34">
         <v>62</v>
       </c>
@@ -6412,7 +6507,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="34">
         <v>63</v>
       </c>
@@ -6446,7 +6541,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="34">
         <v>64</v>
       </c>
@@ -6480,7 +6575,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A66" s="34">
         <v>65</v>
       </c>
@@ -6514,7 +6609,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="34">
         <v>66</v>
       </c>
@@ -6548,7 +6643,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="34">
         <v>67</v>
       </c>
@@ -6582,7 +6677,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A69" s="34">
         <v>68</v>
       </c>
@@ -6616,7 +6711,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A70" s="34">
         <v>69</v>
       </c>
@@ -6650,7 +6745,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A71" s="34">
         <v>70</v>
       </c>
@@ -6684,7 +6779,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A72" s="34">
         <v>71</v>
       </c>
@@ -6718,7 +6813,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="34">
         <v>72</v>
       </c>
@@ -6752,7 +6847,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="129" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A74" s="34">
         <v>73</v>
       </c>
@@ -6786,7 +6881,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="128" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="34">
         <v>74</v>
       </c>
@@ -6837,16 +6932,16 @@
         <v>161</v>
       </c>
       <c r="F76" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G76" s="38" t="s">
-        <v>395</v>
+        <v>363</v>
       </c>
       <c r="H76" s="38" t="s">
-        <v>396</v>
+        <v>352</v>
       </c>
       <c r="I76" s="38" t="s">
-        <v>397</v>
+        <v>364</v>
       </c>
       <c r="J76" s="39" t="s">
         <v>84</v>
@@ -6859,18 +6954,18 @@
         <v>84</v>
       </c>
       <c r="N76" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O76" s="39" t="s">
         <v>84</v>
       </c>
       <c r="P76" s="42" t="s">
-        <v>400</v>
+        <v>351</v>
       </c>
       <c r="Q76" s="39"/>
       <c r="R76" s="42"/>
       <c r="S76" s="46" t="s">
-        <v>398</v>
+        <v>347</v>
       </c>
       <c r="T76" s="44" t="s">
         <v>330</v>
@@ -6893,16 +6988,16 @@
         <v>163</v>
       </c>
       <c r="F77" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G77" s="38" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="H77" s="38" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="I77" s="38" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="J77" s="39" t="s">
         <v>84</v>
@@ -6915,13 +7010,13 @@
         <v>84</v>
       </c>
       <c r="N77" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O77" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P77" s="39" t="s">
-        <v>400</v>
+      <c r="P77" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q77" s="39"/>
       <c r="R77" s="42"/>
@@ -6947,16 +7042,16 @@
         <v>165</v>
       </c>
       <c r="F78" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G78" s="38" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="H78" s="38" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="I78" s="38" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="J78" s="39" t="s">
         <v>84</v>
@@ -6969,13 +7064,13 @@
         <v>84</v>
       </c>
       <c r="N78" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O78" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P78" s="39" t="s">
-        <v>400</v>
+      <c r="P78" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q78" s="39"/>
       <c r="R78" s="42"/>
@@ -7001,16 +7096,16 @@
         <v>167</v>
       </c>
       <c r="F79" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G79" s="38" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="H79" s="38" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="I79" s="38" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="J79" s="39" t="s">
         <v>84</v>
@@ -7023,13 +7118,13 @@
         <v>84</v>
       </c>
       <c r="N79" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O79" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P79" s="39" t="s">
-        <v>400</v>
+      <c r="P79" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q79" s="39"/>
       <c r="R79" s="42"/>
@@ -7055,16 +7150,16 @@
         <v>169</v>
       </c>
       <c r="F80" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G80" s="38" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="H80" s="38" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="I80" s="38" t="s">
-        <v>373</v>
+        <v>379</v>
       </c>
       <c r="J80" s="39" t="s">
         <v>84</v>
@@ -7077,13 +7172,13 @@
         <v>84</v>
       </c>
       <c r="N80" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O80" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P80" s="39" t="s">
-        <v>400</v>
+      <c r="P80" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q80" s="39"/>
       <c r="R80" s="42"/>
@@ -7109,7 +7204,7 @@
         <v>171</v>
       </c>
       <c r="F81" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G81" s="38" t="s">
         <v>375</v>
@@ -7131,13 +7226,13 @@
         <v>84</v>
       </c>
       <c r="N81" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O81" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P81" s="39" t="s">
-        <v>400</v>
+      <c r="P81" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q81" s="39"/>
       <c r="R81" s="42"/>
@@ -7163,16 +7258,16 @@
         <v>173</v>
       </c>
       <c r="F82" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G82" s="38" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="H82" s="38" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="I82" s="38" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J82" s="39" t="s">
         <v>84</v>
@@ -7185,13 +7280,13 @@
         <v>84</v>
       </c>
       <c r="N82" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O82" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P82" s="39" t="s">
-        <v>400</v>
+      <c r="P82" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q82" s="39"/>
       <c r="R82" s="42"/>
@@ -7217,16 +7312,16 @@
         <v>175</v>
       </c>
       <c r="F83" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G83" s="38" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="H83" s="38" t="s">
-        <v>380</v>
+        <v>396</v>
       </c>
       <c r="I83" s="38" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="J83" s="39" t="s">
         <v>84</v>
@@ -7239,13 +7334,13 @@
         <v>84</v>
       </c>
       <c r="N83" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O83" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P83" s="39" t="s">
-        <v>400</v>
+      <c r="P83" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q83" s="39"/>
       <c r="R83" s="42"/>
@@ -7271,16 +7366,16 @@
         <v>177</v>
       </c>
       <c r="F84" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G84" s="38" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="H84" s="38" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="I84" s="38" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="J84" s="39" t="s">
         <v>84</v>
@@ -7293,13 +7388,13 @@
         <v>84</v>
       </c>
       <c r="N84" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O84" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P84" s="39" t="s">
-        <v>400</v>
+      <c r="P84" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q84" s="39"/>
       <c r="R84" s="42"/>
@@ -7325,16 +7420,16 @@
         <v>179</v>
       </c>
       <c r="F85" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G85" s="38" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="H85" s="38" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="I85" s="38" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="J85" s="39" t="s">
         <v>84</v>
@@ -7347,13 +7442,13 @@
         <v>84</v>
       </c>
       <c r="N85" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O85" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P85" s="39" t="s">
-        <v>400</v>
+      <c r="P85" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q85" s="39"/>
       <c r="R85" s="42"/>
@@ -7379,16 +7474,16 @@
         <v>181</v>
       </c>
       <c r="F86" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G86" s="38" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="H86" s="38" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="I86" s="38" t="s">
-        <v>391</v>
+        <v>397</v>
       </c>
       <c r="J86" s="39" t="s">
         <v>84</v>
@@ -7401,13 +7496,13 @@
         <v>84</v>
       </c>
       <c r="N86" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O86" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P86" s="39" t="s">
-        <v>400</v>
+      <c r="P86" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q86" s="39"/>
       <c r="R86" s="42"/>
@@ -7416,7 +7511,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A87" s="34">
         <v>86</v>
       </c>
@@ -7440,7 +7535,7 @@
         <v>321</v>
       </c>
       <c r="K87" s="39" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L87" s="39"/>
       <c r="M87" s="39" t="s">
@@ -7456,7 +7551,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="145" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" ht="241" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A88" s="34">
         <v>87</v>
       </c>
@@ -7480,7 +7575,7 @@
         <v>321</v>
       </c>
       <c r="K88" s="39" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="L88" s="39"/>
       <c r="M88" s="39" t="s">
@@ -7496,7 +7591,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="34">
         <v>88</v>
       </c>
@@ -7520,7 +7615,7 @@
         <v>321</v>
       </c>
       <c r="K89" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L89" s="39"/>
       <c r="M89" s="39" t="s">
@@ -7536,7 +7631,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" ht="209" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A90" s="34">
         <v>89</v>
       </c>
@@ -7560,7 +7655,7 @@
         <v>321</v>
       </c>
       <c r="K90" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L90" s="39"/>
       <c r="M90" s="39" t="s">
@@ -7576,7 +7671,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="91" spans="1:20" ht="113" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" ht="209" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A91" s="34">
         <v>90</v>
       </c>
@@ -7600,7 +7695,7 @@
         <v>321</v>
       </c>
       <c r="K91" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L91" s="39"/>
       <c r="M91" s="39" t="s">
@@ -7616,7 +7711,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A92" s="34">
         <v>91</v>
       </c>
@@ -7640,7 +7735,7 @@
         <v>321</v>
       </c>
       <c r="K92" s="39" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="L92" s="39"/>
       <c r="M92" s="39" t="s">
@@ -7656,7 +7751,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="129" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" ht="225" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A93" s="34">
         <v>92</v>
       </c>
@@ -7680,7 +7775,7 @@
         <v>321</v>
       </c>
       <c r="K93" s="39" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L93" s="39"/>
       <c r="M93" s="39" t="s">
@@ -7713,16 +7808,16 @@
         <v>197</v>
       </c>
       <c r="F94" s="37">
-        <v>44981</v>
+        <v>45027</v>
       </c>
       <c r="G94" s="38" t="s">
+        <v>394</v>
+      </c>
+      <c r="H94" s="38" t="s">
         <v>393</v>
       </c>
-      <c r="H94" s="38" t="s">
-        <v>392</v>
-      </c>
       <c r="I94" s="38" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="J94" s="39" t="s">
         <v>84</v>
@@ -7735,13 +7830,13 @@
         <v>84</v>
       </c>
       <c r="N94" s="39" t="s">
-        <v>401</v>
+        <v>350</v>
       </c>
       <c r="O94" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="P94" s="39" t="s">
-        <v>400</v>
+      <c r="P94" s="42" t="s">
+        <v>351</v>
       </c>
       <c r="Q94" s="39"/>
       <c r="R94" s="42"/>
@@ -7750,7 +7845,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:20" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="34">
         <v>94</v>
       </c>
@@ -7784,7 +7879,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:20" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="34">
         <v>95</v>
       </c>
@@ -7818,7 +7913,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="34">
         <v>96</v>
       </c>
@@ -7852,7 +7947,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="34">
         <v>97</v>
       </c>
@@ -7886,7 +7981,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:20" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="34">
         <v>98</v>
       </c>
@@ -7920,7 +8015,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:20" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="34">
         <v>99</v>
       </c>
@@ -7954,7 +8049,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="34">
         <v>100</v>
       </c>
@@ -7988,7 +8083,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="34">
         <v>101</v>
       </c>
@@ -8022,7 +8117,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:20" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="34">
         <v>102</v>
       </c>
@@ -8056,7 +8151,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:20" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="34">
         <v>103</v>
       </c>
@@ -8090,7 +8185,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="34">
         <v>104</v>
       </c>
@@ -8124,7 +8219,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:20" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="34">
         <v>105</v>
       </c>
@@ -8158,7 +8253,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="144" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:20" ht="256" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="34">
         <v>106</v>
       </c>
@@ -8192,7 +8287,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="34">
         <v>107</v>
       </c>
@@ -8226,7 +8321,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="34">
         <v>108</v>
       </c>
@@ -8260,7 +8355,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="34">
         <v>109</v>
       </c>
@@ -8294,7 +8389,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="34">
         <v>110</v>
       </c>
@@ -8328,7 +8423,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="34">
         <v>111</v>
       </c>
@@ -8362,7 +8457,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="34">
         <v>112</v>
       </c>
@@ -8396,7 +8491,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="34">
         <v>113</v>
       </c>
@@ -8430,7 +8525,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="34">
         <v>114</v>
       </c>
@@ -8464,7 +8559,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="116" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="34">
         <v>115</v>
       </c>
@@ -8498,7 +8593,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="34">
         <v>116</v>
       </c>
@@ -8532,7 +8627,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="34">
         <v>117</v>
       </c>
@@ -8566,7 +8661,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="34">
         <v>118</v>
       </c>
@@ -8600,7 +8695,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="120" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="34">
         <v>119</v>
       </c>
@@ -8634,7 +8729,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="121" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="34">
         <v>120</v>
       </c>
@@ -8668,7 +8763,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="122" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:20" ht="240" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="34">
         <v>121</v>
       </c>
@@ -8702,7 +8797,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="34">
         <v>122</v>
       </c>
@@ -8736,7 +8831,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="34">
         <v>123</v>
       </c>
@@ -8770,7 +8865,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="34">
         <v>124</v>
       </c>
@@ -8804,7 +8899,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="34">
         <v>125</v>
       </c>
@@ -8838,7 +8933,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="34">
         <v>126</v>
       </c>
@@ -8872,7 +8967,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="34">
         <v>127</v>
       </c>
@@ -8906,7 +9001,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="129" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="34">
         <v>128</v>
       </c>
@@ -8940,7 +9035,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="34">
         <v>129</v>
       </c>
@@ -8974,7 +9069,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="131" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="34">
         <v>130</v>
       </c>
@@ -9008,7 +9103,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="132" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="34">
         <v>131</v>
       </c>
@@ -9042,7 +9137,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="133" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="34">
         <v>132</v>
       </c>
@@ -9076,7 +9171,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="134" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="34">
         <v>133</v>
       </c>
@@ -9110,7 +9205,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="34">
         <v>134</v>
       </c>
@@ -9144,7 +9239,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="34">
         <v>135</v>
       </c>
@@ -9178,7 +9273,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="34">
         <v>136</v>
       </c>
@@ -9212,7 +9307,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="34">
         <v>137</v>
       </c>
@@ -9246,7 +9341,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="34">
         <v>138</v>
       </c>
@@ -9280,7 +9375,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="140" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="34">
         <v>139</v>
       </c>
@@ -9314,7 +9409,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="141" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="34">
         <v>140</v>
       </c>
@@ -9348,7 +9443,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="34">
         <v>141</v>
       </c>
@@ -9382,7 +9477,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="143" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="34">
         <v>142</v>
       </c>
@@ -9416,7 +9511,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="144" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="34">
         <v>143</v>
       </c>
@@ -9450,7 +9545,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="145" spans="1:20" ht="112" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:20" ht="208" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="34">
         <v>144</v>
       </c>
@@ -9484,7 +9579,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="146" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="34">
         <v>145</v>
       </c>
@@ -9518,7 +9613,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="147" spans="1:20" ht="128" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:20" ht="224" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" s="34">
         <v>146</v>
       </c>
@@ -23956,7 +24051,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O10:O1048576 O1:O8 L1:M8 L10:M1048576</xm:sqref>
+          <xm:sqref>O1:O8 L1:M8 O95:O1048576 O10:O36 L10:M36 L38:L42 L44:L48 L50:L75 M59:M75 O59:O75 O87:O93 L87:M93 L95:M1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -26125,6 +26220,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -26355,7 +26459,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
@@ -26366,16 +26470,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26394,7 +26497,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
@@ -26411,14 +26514,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
A1#111FUJIFILM000 Correzione token jwt
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/accreditamento-checklist_V4.2.xlsx
+++ b/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/accreditamento-checklist_V4.2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmontel/Documents/dev/FSE/it-fse-accreditamento/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Workflow/4.33/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mmontel/Documents/dev/FSE/it-fse-accreditamento/GATEWAY/A1#111FUJIFILM000/Fujifilm_Italia_S.p.A./Synapse_Value/1.6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A9B316-DF48-7743-B8B2-59120A0BB13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB276E36-201A-AB4A-B370-E4C6B589155E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3240" yWindow="-21100" windowWidth="30980" windowHeight="19700" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1942,148 +1942,148 @@
     <t>Il caso viene gestito in back office con il seguente flusso: 1. Il record di refertazione viene bloccato sull'applicativo in uno stato di manutenzione. 2. Il caso di errore viene visualizzato nel modulo integrato gestione problematiche. 3. Un utente amministratore gestisce il caso, ed una volta risolto, il record di refertazione viene sbloccato e rimosso lo stato di manutenzione. 4. Il medico riceve una notifica automatica che riporta il problema risolto e lo invita a creare e firmare un addendum.</t>
   </si>
   <si>
-    <t>0aa8a2dba0809f3b</t>
-  </si>
-  <si>
-    <t>1913b3b338cd52b6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.7181aa9472^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:21:00.216Z[UTC]</t>
-  </si>
-  <si>
-    <t>d42e7ede64b233fa</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:21:01.112Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.ec2538749c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>888cec3db845d0ad</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:41.589Z[UTC]</t>
-  </si>
-  <si>
-    <t>26f74d71e737ffef</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:59.317Z[UTC]</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:39.974Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.b7aa33d2df^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>02f6c974efb65bfb</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:43.03Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.3ffdacb4e8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>0a02c5f2c87933c7</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:44.48Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.6b1340eecf^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>431c9c23de42236b</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:45.951Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.56b18f0ec4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>56ac2bc544261824</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:49.031Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.ecc1e2b6d2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>068e88e8c55ae948</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:47.532Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.93961c8bc9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>f320be9ee5698d0e</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:50.515Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.bc6f3ba2cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:51.907Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.a27d859a2d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5ff992ade30f769b</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:53.469Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.5eb7049956^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5d2a9cd381bb186d</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:54.915Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.1606281359^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2d2fb460d14af10e</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:56.441Z[UTC]</t>
-  </si>
-  <si>
-    <t>7681f7c242538a52</t>
-  </si>
-  <si>
-    <t>2023-04-11T14:20:57.889Z[UTC]</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.a3139809b3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>5a6c7cf5e8fb7a90</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.e439bcbd28^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>subject_application_id: Synapse Value</t>
   </si>
   <si>
     <t>subject_application_version: 1.6</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:54.786Z[UTC]</t>
+  </si>
+  <si>
+    <t>73d01a0c452d8cbd</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.c04fd843ac^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>cce754078ad956d3</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:55.853Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.377c687be9^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>b93670d555473b9f</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:35.684Z[UTC]</t>
+  </si>
+  <si>
+    <t>01a44b13e4b83ec3</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:53.796Z[UTC]</t>
+  </si>
+  <si>
+    <t>618b0a2cc2dfe936</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:33.754Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.82befc22e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>20c2a4e7b34c2af8</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:37.223Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.a966b48ca0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8127e05c5a0bceec</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:38.75Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.569b853d6f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>857e3b18c0c24907</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:40.392Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.c94cc7a2d3^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>0ef93cc283f026f7</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:41.928Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.66b4be7fe5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>39f134f721de69bd</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:43.669Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.1d04bb6000^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>8e941b093d2661d6</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:45.18Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.b44b93f95a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>eb43f87a7f603264</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:46.663Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.8f12c5f594^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>dae6e03ada103e3d</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:48.174Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.74c052a195^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>27c647eb58db4229</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:49.591Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.406017ac42^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>9c3180e838448e6a</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:51.044Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.8e90bed842^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>ad75d555897fc0fc</t>
+  </si>
+  <si>
+    <t>2023-04-17T13:49:52.475Z[UTC]</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.4.1.3.7743.b858460b54cc28b3e4e9c5f50b36baf44ccec41b1051d4a9f9ff662e194e6257.6345556ec2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2578,7 +2578,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2753,6 +2753,10 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -4202,11 +4206,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:T992"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="F19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5:D5"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4217,8 +4221,8 @@
     <col min="4" max="4" width="44.1640625" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="46.33203125" style="25" customWidth="1"/>
     <col min="6" max="6" width="25.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5" style="25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.83203125" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" style="25" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" style="25" customWidth="1"/>
     <col min="9" max="9" width="31.83203125" style="25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.83203125" style="25" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="37.6640625" style="25" bestFit="1" customWidth="1"/>
@@ -4282,7 +4286,7 @@
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="58" t="s">
-        <v>398</v>
+        <v>352</v>
       </c>
       <c r="D3" s="50"/>
       <c r="F3" s="26"/>
@@ -4329,7 +4333,7 @@
       <c r="A5" s="56"/>
       <c r="B5" s="57"/>
       <c r="C5" s="58" t="s">
-        <v>399</v>
+        <v>353</v>
       </c>
       <c r="D5" s="50"/>
       <c r="F5" s="26"/>
@@ -4637,7 +4641,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="34">
         <v>6</v>
       </c>
@@ -4671,7 +4675,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="34">
         <v>7</v>
       </c>
@@ -4705,7 +4709,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34">
         <v>8</v>
       </c>
@@ -4739,7 +4743,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34">
         <v>9</v>
       </c>
@@ -4790,16 +4794,16 @@
         <v>48</v>
       </c>
       <c r="F19" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G19" s="38" t="s">
+        <v>354</v>
+      </c>
+      <c r="H19" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="H19" s="38" t="s">
-        <v>353</v>
-      </c>
       <c r="I19" s="38" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="J19" s="39" t="s">
         <v>84</v>
@@ -4834,16 +4838,16 @@
         <v>50</v>
       </c>
       <c r="F20" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G20" s="38" t="s">
+        <v>358</v>
+      </c>
+      <c r="H20" s="38" t="s">
         <v>357</v>
       </c>
-      <c r="H20" s="38" t="s">
-        <v>356</v>
-      </c>
       <c r="I20" s="38" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="J20" s="39" t="s">
         <v>84</v>
@@ -5073,7 +5077,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="34">
         <v>20</v>
       </c>
@@ -5107,7 +5111,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="34">
         <v>21</v>
       </c>
@@ -5141,7 +5145,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="34">
         <v>22</v>
       </c>
@@ -5175,7 +5179,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="289" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" ht="273" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="34">
         <v>23</v>
       </c>
@@ -5413,7 +5417,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="257" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" ht="241" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="34">
         <v>31</v>
       </c>
@@ -5430,13 +5434,13 @@
         <v>88</v>
       </c>
       <c r="F37" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G37" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="H37" s="38" t="s">
         <v>360</v>
-      </c>
-      <c r="H37" s="38" t="s">
-        <v>359</v>
       </c>
       <c r="I37" s="38" t="s">
         <v>346</v>
@@ -5677,7 +5681,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="257" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="241" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="34">
         <v>39</v>
       </c>
@@ -5694,13 +5698,13 @@
         <v>100</v>
       </c>
       <c r="F43" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G43" s="38" t="s">
+        <v>363</v>
+      </c>
+      <c r="H43" s="38" t="s">
         <v>362</v>
-      </c>
-      <c r="H43" s="38" t="s">
-        <v>361</v>
       </c>
       <c r="I43" s="38" t="s">
         <v>346</v>
@@ -5962,7 +5966,7 @@
         <v>108</v>
       </c>
       <c r="F49" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G49" s="38"/>
       <c r="H49" s="38"/>
@@ -6259,7 +6263,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="34">
         <v>56</v>
       </c>
@@ -6337,7 +6341,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="34">
         <v>58</v>
       </c>
@@ -6371,7 +6375,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="34">
         <v>59</v>
       </c>
@@ -6405,7 +6409,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="34">
         <v>60</v>
       </c>
@@ -6439,7 +6443,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="34">
         <v>61</v>
       </c>
@@ -6473,7 +6477,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="241" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" ht="225" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="34">
         <v>62</v>
       </c>
@@ -6915,7 +6919,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A76" s="34">
         <v>75</v>
       </c>
@@ -6932,16 +6936,16 @@
         <v>161</v>
       </c>
       <c r="F76" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G76" s="38" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="H76" s="38" t="s">
-        <v>352</v>
+        <v>364</v>
       </c>
       <c r="I76" s="38" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="J76" s="39" t="s">
         <v>84</v>
@@ -6971,7 +6975,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A77" s="34">
         <v>76</v>
       </c>
@@ -6988,16 +6992,16 @@
         <v>163</v>
       </c>
       <c r="F77" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G77" s="38" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="H77" s="38" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="I77" s="38" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="J77" s="39" t="s">
         <v>84</v>
@@ -7025,7 +7029,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A78" s="34">
         <v>77</v>
       </c>
@@ -7042,16 +7046,16 @@
         <v>165</v>
       </c>
       <c r="F78" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G78" s="38" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="H78" s="38" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="I78" s="38" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="J78" s="39" t="s">
         <v>84</v>
@@ -7079,7 +7083,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A79" s="34">
         <v>78</v>
       </c>
@@ -7096,16 +7100,16 @@
         <v>167</v>
       </c>
       <c r="F79" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G79" s="38" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="H79" s="38" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="I79" s="38" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="J79" s="39" t="s">
         <v>84</v>
@@ -7133,7 +7137,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A80" s="34">
         <v>79</v>
       </c>
@@ -7150,16 +7154,16 @@
         <v>169</v>
       </c>
       <c r="F80" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G80" s="38" t="s">
+        <v>377</v>
+      </c>
+      <c r="H80" s="38" t="s">
+        <v>376</v>
+      </c>
+      <c r="I80" s="38" t="s">
         <v>378</v>
-      </c>
-      <c r="H80" s="38" t="s">
-        <v>377</v>
-      </c>
-      <c r="I80" s="38" t="s">
-        <v>379</v>
       </c>
       <c r="J80" s="39" t="s">
         <v>84</v>
@@ -7187,7 +7191,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A81" s="34">
         <v>80</v>
       </c>
@@ -7204,16 +7208,16 @@
         <v>171</v>
       </c>
       <c r="F81" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G81" s="38" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="H81" s="38" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="I81" s="38" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="J81" s="39" t="s">
         <v>84</v>
@@ -7241,7 +7245,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A82" s="34">
         <v>81</v>
       </c>
@@ -7258,16 +7262,16 @@
         <v>173</v>
       </c>
       <c r="F82" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G82" s="38" t="s">
-        <v>381</v>
-      </c>
-      <c r="H82" s="38" t="s">
-        <v>380</v>
+        <v>383</v>
+      </c>
+      <c r="H82" s="59" t="s">
+        <v>382</v>
       </c>
       <c r="I82" s="38" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="J82" s="39" t="s">
         <v>84</v>
@@ -7295,7 +7299,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A83" s="34">
         <v>82</v>
       </c>
@@ -7312,16 +7316,16 @@
         <v>175</v>
       </c>
       <c r="F83" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G83" s="38" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="H83" s="38" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="I83" s="38" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="J83" s="39" t="s">
         <v>84</v>
@@ -7349,7 +7353,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A84" s="34">
         <v>83</v>
       </c>
@@ -7366,16 +7370,16 @@
         <v>177</v>
       </c>
       <c r="F84" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G84" s="38" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="H84" s="38" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="I84" s="38" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="J84" s="39" t="s">
         <v>84</v>
@@ -7403,7 +7407,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A85" s="34">
         <v>84</v>
       </c>
@@ -7420,16 +7424,16 @@
         <v>179</v>
       </c>
       <c r="F85" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G85" s="38" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="H85" s="38" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="I85" s="38" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="J85" s="39" t="s">
         <v>84</v>
@@ -7457,7 +7461,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="289" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" ht="273" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A86" s="34">
         <v>85</v>
       </c>
@@ -7474,16 +7478,16 @@
         <v>181</v>
       </c>
       <c r="F86" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G86" s="38" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="H86" s="38" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="I86" s="38" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J86" s="39" t="s">
         <v>84</v>
@@ -7791,7 +7795,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="288" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:20" ht="272" x14ac:dyDescent="0.2">
       <c r="A94" s="34">
         <v>93</v>
       </c>
@@ -7808,16 +7812,16 @@
         <v>197</v>
       </c>
       <c r="F94" s="37">
-        <v>45027</v>
+        <v>45033</v>
       </c>
       <c r="G94" s="38" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="H94" s="38" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="I94" s="38" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="J94" s="39" t="s">
         <v>84</v>
@@ -26229,6 +26233,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b4730850ec8220df2460bf5d75163141">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c2168c1cf3d5a08369735c09b24c7b76" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -26459,17 +26474,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3F02EBF-A415-4FB6-A4E4-A6920890B7C4}">
   <ds:schemaRefs>
@@ -26479,6 +26483,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6395DAD-5B77-46ED-9147-4C5A384B6E5B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26497,23 +26518,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAC13FE-B745-460A-BC76-FAEE62F3EBA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>